<commit_message>
Se genero la clase Aula y la carga de Aulas
</commit_message>
<xml_diff>
--- a/Tablas.xlsx
+++ b/Tablas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="6120" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Materia" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Codigo Materia</t>
-  </si>
-  <si>
-    <t>Codigo Aula</t>
   </si>
   <si>
     <t>Codigo Facultad</t>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Lic. en Diseño Indumentaria y Textil</t>
+  </si>
+  <si>
+    <t>CodigoAula</t>
   </si>
 </sst>
 </file>
@@ -640,25 +640,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -672,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -12787,7 +12787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -12798,16 +12800,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -12821,7 +12823,7 @@
         <v>180</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -12835,7 +12837,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -12849,7 +12851,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12863,7 +12865,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12877,7 +12879,7 @@
         <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12891,7 +12893,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12905,7 +12907,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12919,7 +12921,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12933,7 +12935,7 @@
         <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -12947,7 +12949,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -12961,7 +12963,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -12975,7 +12977,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -12989,7 +12991,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -13003,7 +13005,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -13017,7 +13019,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -13031,7 +13033,7 @@
         <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -13045,7 +13047,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -13059,7 +13061,7 @@
         <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -13073,7 +13075,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
@@ -13087,7 +13089,7 @@
         <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
@@ -13101,7 +13103,7 @@
         <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
@@ -13115,7 +13117,7 @@
         <v>56</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
@@ -13129,7 +13131,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
@@ -13143,7 +13145,7 @@
         <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
@@ -13157,7 +13159,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
@@ -13171,7 +13173,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
@@ -13185,7 +13187,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
@@ -13199,7 +13201,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
@@ -13213,7 +13215,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
@@ -13227,7 +13229,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
@@ -13241,7 +13243,7 @@
         <v>36</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
@@ -13255,7 +13257,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
@@ -13269,7 +13271,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
@@ -13283,7 +13285,7 @@
         <v>16</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
@@ -13297,7 +13299,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
@@ -13311,7 +13313,7 @@
         <v>66</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
@@ -13325,7 +13327,7 @@
         <v>110</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1">
@@ -13339,7 +13341,7 @@
         <v>200</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
@@ -13353,7 +13355,7 @@
         <v>20</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
@@ -13367,7 +13369,7 @@
         <v>30</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
@@ -13381,7 +13383,7 @@
         <v>109</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
@@ -13395,7 +13397,7 @@
         <v>90</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
@@ -13409,7 +13411,7 @@
         <v>110</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">
@@ -19158,7 +19160,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -19169,10 +19173,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -19180,7 +19184,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -19188,7 +19192,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -19196,7 +19200,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -19204,7 +19208,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -19212,7 +19216,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -23213,16 +23217,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -23233,7 +23237,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2">
         <v>59</v>
@@ -23247,7 +23251,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="2">
         <v>38</v>
@@ -23261,7 +23265,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2">
         <v>38</v>
@@ -23275,7 +23279,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2">
         <v>35</v>
@@ -23289,7 +23293,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="2">
         <v>15</v>
@@ -23303,7 +23307,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2">
         <v>14</v>
@@ -23317,7 +23321,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2">
         <v>41</v>
@@ -23331,7 +23335,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2">
         <v>41</v>
@@ -23345,7 +23349,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2">
         <v>47</v>
@@ -23359,7 +23363,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2">
         <v>44</v>
@@ -23373,7 +23377,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2">
         <v>9</v>
@@ -23387,7 +23391,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2">
         <v>33</v>
@@ -23401,7 +23405,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2">
         <v>69</v>
@@ -23415,7 +23419,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2">
         <v>34</v>
@@ -23429,7 +23433,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2">
         <v>39</v>

</xml_diff>